<commit_message>
Implement slide_tissue manifest; full tests for both manifests
</commit_message>
<xml_diff>
--- a/tests/models/templates/examples/pbmc_manifest.xlsx
+++ b/tests/models/templates/examples/pbmc_manifest.xlsx
@@ -1895,10 +1895,10 @@
   <dimension ref="B1:D65"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C3 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="2" style="0" width="30.66"/>
   </cols>
@@ -2569,10 +2569,10 @@
   <dimension ref="A1:U18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C3 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="2" style="0" width="30.66"/>
   </cols>
@@ -3158,10 +3158,10 @@
   <dimension ref="A1:C2018"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="1" style="0" width="30.66"/>
   </cols>
@@ -13362,10 +13362,10 @@
   <dimension ref="A1:O2004"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="1" sqref="C3 B5"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="1" style="0" width="30.66"/>
   </cols>
@@ -23767,10 +23767,10 @@
   <dimension ref="A1:AB2004"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="1" sqref="C3 G5"/>
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="1" style="0" width="30.66"/>
   </cols>

</xml_diff>

<commit_message>
CIDC-1067 some perfecting tweaks
</commit_message>
<xml_diff>
--- a/tests/models/templates/examples/pbmc_manifest.xlsx
+++ b/tests/models/templates/examples/pbmc_manifest.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="1" state="visible" r:id="rId2"/>
@@ -889,7 +889,7 @@
     <t xml:space="preserve">Section 'Path Concordance Verification' of tab 'Essential Patient Data'</t>
   </si>
   <si>
-    <t xml:space="preserve">participant id</t>
+    <t xml:space="preserve">trial participant id</t>
   </si>
   <si>
     <t xml:space="preserve">Trial Participant Identifier. Crypto-hashed after upload.</t>
@@ -913,7 +913,7 @@
     <t xml:space="preserve">A unique identifier so someone can find the clinical report.</t>
   </si>
   <si>
-    <t xml:space="preserve">event name</t>
+    <t xml:space="preserve">collection event name</t>
   </si>
   <si>
     <t xml:space="preserve">diagnosis verification</t>
@@ -1782,7 +1782,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1813,6 +1813,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1894,11 +1898,11 @@
   </sheetPr>
   <dimension ref="B1:D65"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E29" activeCellId="1" sqref="G6:G10 E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="2" style="0" width="30.66"/>
   </cols>
@@ -2121,7 +2125,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="4" t="s">
         <v>43</v>
       </c>
@@ -2259,7 +2263,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="4" t="s">
         <v>43</v>
       </c>
@@ -2569,10 +2573,10 @@
   <dimension ref="A1:U18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="G6:G10 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="2" style="0" width="30.66"/>
   </cols>
@@ -3157,11 +3161,11 @@
   </sheetPr>
   <dimension ref="A1:C2018"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B18" activeCellId="1" sqref="G6:G10 B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="1" style="0" width="30.66"/>
   </cols>
@@ -3334,7 +3338,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>237</v>
       </c>
@@ -13361,13 +13365,13 @@
   </sheetPr>
   <dimension ref="A1:O2004"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6:G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="1" style="0" width="30.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="1" style="0" width="30.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13451,7 +13455,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>238</v>
       </c>
@@ -13470,7 +13474,7 @@
       <c r="F5" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="8" t="s">
         <v>248</v>
       </c>
       <c r="H5" s="0" t="s">
@@ -13498,7 +13502,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>238</v>
       </c>
@@ -13517,7 +13521,7 @@
       <c r="F6" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="8" t="s">
         <v>248</v>
       </c>
       <c r="H6" s="0" t="s">
@@ -13545,7 +13549,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>238</v>
       </c>
@@ -13564,7 +13568,7 @@
       <c r="F7" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="8" t="s">
         <v>248</v>
       </c>
       <c r="H7" s="0" t="s">
@@ -13592,7 +13596,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>238</v>
       </c>
@@ -13611,7 +13615,7 @@
       <c r="F8" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="8" t="s">
         <v>248</v>
       </c>
       <c r="H8" s="0" t="s">
@@ -13639,7 +13643,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>238</v>
       </c>
@@ -13658,7 +13662,7 @@
       <c r="F9" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="8" t="s">
         <v>248</v>
       </c>
       <c r="H9" s="0" t="s">
@@ -13686,7 +13690,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>238</v>
       </c>
@@ -13705,7 +13709,7 @@
       <c r="F10" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="8" t="s">
         <v>248</v>
       </c>
       <c r="H10" s="0" t="s">
@@ -23710,50 +23714,46 @@
     <mergeCell ref="H3:L3"/>
     <mergeCell ref="M3:O3"/>
   </mergeCells>
-  <dataValidations count="9">
-    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="O5:O10" type="list">
-      <formula1>"Hispanic or Latino,Not Hispanic or Latino,Not reported,Unknown,Other"</formula1>
+  <dataValidations count="8">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G11:G2004" type="list">
+      <formula1>'Data Dictionary'!$G$2:$G$6</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="M11:M2004" type="list">
+      <formula1>'Data Dictionary'!$H$2:$H$5</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="N11:N2004" type="list">
+      <formula1>'Data Dictionary'!$I$2:$I$9</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="O11:O2004" type="list">
+      <formula1>'Data Dictionary'!$J$2:$J$6</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F5:F10" type="list">
+      <formula1>"Baseline,Pre_Day_1_Cycle_2,Restaging,Off_study,Cycle_2_Week_3,Cycle_4_Week_7,Cycle_5_Week_9,Progression,Cycle_3,End_of_treatment,On_Treatment,Response,Relapse,Day_8,Cycle_2_Day_1,T0,T1,T2,T3,T4,T5,T6,End_of_Treatment,Progression,Other,Not_reported"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="M5:M10" type="list">
+      <formula1>"Male,Female,Not Specified,Other"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="N5:N10" type="list">
       <formula1>"American Indian/Alaska Native,Asian,Black/African American,Native Hawaiian/Pacific Islander,White,Not Reported,Unknown,Other"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="M5:M10" type="list">
-      <formula1>"Male,Female,Not Specified,Other"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G5:G10" type="list">
-      <formula1>"Local pathology review was not consistent,Local pathology review was consistent with site of tissue procurement diagnostic pathology report,Not Available,Not Reported,Other"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F5:F10" type="list">
-      <formula1>"Baseline,Pre_Day_1_Cycle_2,Restaging,Off_study,Cycle_2_Week_3,Cycle_4_Week_7,Cycle_5_Week_9,Progression,Cycle_3,End_of_treatment,On_Treatment,Response,Relapse,Day_8,Cycle_2_Day_1,T0,T1,T2,T3,T4,T5,T6,End_of_Treatment,Progression,Other,Not_reported"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F11 G12:G2004" type="list">
-      <formula1>'Data Dictionary'!$G$2:$G$6</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="L11 M12:M2004" type="list">
-      <formula1>'Data Dictionary'!$H$2:$H$5</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="M11 N12:N2004" type="list">
-      <formula1>'Data Dictionary'!$I$2:$I$9</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="N11 O12:O2004" type="list">
-      <formula1>'Data Dictionary'!$J$2:$J$6</formula1>
+    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="O5:O10" type="list">
+      <formula1>"Hispanic or Latino,Not Hispanic or Latino,Not reported,Unknown,Other"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
@@ -23766,11 +23766,11 @@
   </sheetPr>
   <dimension ref="A1:AB2004"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L4" activeCellId="1" sqref="G6:G10 L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="1" style="0" width="30.66"/>
   </cols>
@@ -23822,7 +23822,7 @@
       <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>237</v>
       </c>

</xml_diff>